<commit_message>
update for BITI link number correction
</commit_message>
<xml_diff>
--- a/BITI_setup_input.xlsx
+++ b/BITI_setup_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madel\Coastal Hydro Dropbox\Madeline Foster-Martinez\MRF_BITI\BITI_2023_code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eric\git\ICM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9B895B-FE8C-4C53-9210-BB7A36233415}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91966C49-8C21-4074-B7F8-EB21B65AF807}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="4050" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -466,7 +469,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -476,18 +479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="14">
         <v>1</v>
       </c>
@@ -504,24 +507,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="15">
-        <v>29</v>
+        <v>906</v>
       </c>
       <c r="C3" s="15">
-        <v>30</v>
+        <v>907</v>
       </c>
       <c r="D3" s="15">
-        <v>31</v>
+        <v>908</v>
       </c>
       <c r="E3" s="15">
-        <v>32</v>
+        <v>909</v>
       </c>
       <c r="F3" s="15">
-        <v>33</v>
+        <v>910</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>3</v>
@@ -530,7 +533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -553,12 +556,12 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>461</v>
       </c>
@@ -582,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>472</v>
       </c>
@@ -606,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>476</v>
       </c>
@@ -630,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>477</v>
       </c>
@@ -654,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>479</v>
       </c>
@@ -678,7 +681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>480</v>
       </c>
@@ -689,22 +692,22 @@
         <v>0</v>
       </c>
       <c r="D11" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="14">
         <v>0</v>
       </c>
       <c r="F11" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B12" s="14">
         <v>0</v>
@@ -713,10 +716,10 @@
         <v>0</v>
       </c>
       <c r="D12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="14">
         <v>0</v>
@@ -726,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>483</v>
       </c>
@@ -750,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>485</v>
       </c>
@@ -774,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>486</v>
       </c>
@@ -798,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>505</v>
       </c>
@@ -822,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>506</v>
       </c>
@@ -846,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>507</v>
       </c>
@@ -870,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>508</v>
       </c>
@@ -894,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>509</v>
       </c>
@@ -918,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>510</v>
       </c>
@@ -942,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>511</v>
       </c>
@@ -966,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>513</v>
       </c>
@@ -990,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>520</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>521</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>529</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>530</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>531</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>532</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>533</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>534</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>535</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>536</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>537</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>538</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>539</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>666</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>667</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>684</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>688</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>694</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>695</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>696</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>697</v>
       </c>
@@ -1494,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>700</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>703</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>708</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>709</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>710</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>711</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>712</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>714</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>715</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>716</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>717</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>718</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>746</v>
       </c>
@@ -1806,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>749</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>750</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>775</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>776</v>
       </c>
@@ -1902,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>834</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>835</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>836</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>837</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>838</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>839</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>858</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>911</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>922</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>923</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>926</v>
       </c>
@@ -2166,7 +2169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>937</v>
       </c>
@@ -2190,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>939</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>942</v>
       </c>
@@ -2248,24 +2251,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A87" workbookViewId="0">
       <selection activeCell="L3" sqref="L3:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" style="7" customWidth="1"/>
-    <col min="7" max="10" width="9.109375" style="7"/>
-    <col min="11" max="11" width="9.109375" style="11"/>
-    <col min="12" max="16384" width="9.109375" style="5"/>
+    <col min="3" max="3" width="6.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="7" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" style="7"/>
+    <col min="11" max="11" width="9.140625" style="11"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2273,7 +2276,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="10">
         <v>1</v>
@@ -2303,7 +2306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -2392,7 +2395,7 @@
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -2418,7 +2421,7 @@
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>148</v>
       </c>
@@ -2470,7 +2473,7 @@
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>149</v>
       </c>
@@ -2522,7 +2525,7 @@
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>150</v>
       </c>
@@ -2574,7 +2577,7 @@
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>151</v>
       </c>
@@ -2626,7 +2629,7 @@
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>152</v>
       </c>
@@ -2678,7 +2681,7 @@
       <c r="AD10" s="7"/>
       <c r="AE10" s="7"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>153</v>
       </c>
@@ -2730,7 +2733,7 @@
       <c r="AD11" s="7"/>
       <c r="AE11" s="7"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>154</v>
       </c>
@@ -2782,7 +2785,7 @@
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>155</v>
       </c>
@@ -2834,7 +2837,7 @@
       <c r="AD13" s="7"/>
       <c r="AE13" s="7"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>156</v>
       </c>
@@ -2886,7 +2889,7 @@
       <c r="AD14" s="7"/>
       <c r="AE14" s="7"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>157</v>
       </c>
@@ -2938,7 +2941,7 @@
       <c r="AD15" s="7"/>
       <c r="AE15" s="7"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>158</v>
       </c>
@@ -2990,7 +2993,7 @@
       <c r="AD16" s="7"/>
       <c r="AE16" s="7"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>164</v>
       </c>
@@ -3042,7 +3045,7 @@
       <c r="AD17" s="7"/>
       <c r="AE17" s="7"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>165</v>
       </c>
@@ -3094,7 +3097,7 @@
       <c r="AD18" s="7"/>
       <c r="AE18" s="7"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>166</v>
       </c>
@@ -3146,7 +3149,7 @@
       <c r="AD19" s="7"/>
       <c r="AE19" s="7"/>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>167</v>
       </c>
@@ -3198,7 +3201,7 @@
       <c r="AD20" s="7"/>
       <c r="AE20" s="7"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>169</v>
       </c>
@@ -3250,7 +3253,7 @@
       <c r="AD21" s="7"/>
       <c r="AE21" s="7"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>170</v>
       </c>
@@ -3302,7 +3305,7 @@
       <c r="AD22" s="7"/>
       <c r="AE22" s="7"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>171</v>
       </c>
@@ -3354,7 +3357,7 @@
       <c r="AD23" s="7"/>
       <c r="AE23" s="7"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>175</v>
       </c>
@@ -3406,7 +3409,7 @@
       <c r="AD24" s="7"/>
       <c r="AE24" s="7"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>176</v>
       </c>
@@ -3458,7 +3461,7 @@
       <c r="AD25" s="7"/>
       <c r="AE25" s="7"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>183</v>
       </c>
@@ -3510,7 +3513,7 @@
       <c r="AD26" s="7"/>
       <c r="AE26" s="7"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>184</v>
       </c>
@@ -3562,7 +3565,7 @@
       <c r="AD27" s="7"/>
       <c r="AE27" s="7"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>185</v>
       </c>
@@ -3614,7 +3617,7 @@
       <c r="AD28" s="7"/>
       <c r="AE28" s="7"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>186</v>
       </c>
@@ -3666,7 +3669,7 @@
       <c r="AD29" s="7"/>
       <c r="AE29" s="7"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>204</v>
       </c>
@@ -3718,7 +3721,7 @@
       <c r="AD30" s="7"/>
       <c r="AE30" s="7"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>205</v>
       </c>
@@ -3770,7 +3773,7 @@
       <c r="AD31" s="7"/>
       <c r="AE31" s="7"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>206</v>
       </c>
@@ -3822,7 +3825,7 @@
       <c r="AD32" s="7"/>
       <c r="AE32" s="7"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>207</v>
       </c>
@@ -3874,7 +3877,7 @@
       <c r="AD33" s="7"/>
       <c r="AE33" s="7"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>208</v>
       </c>
@@ -3926,7 +3929,7 @@
       <c r="AD34" s="7"/>
       <c r="AE34" s="7"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>209</v>
       </c>
@@ -3978,7 +3981,7 @@
       <c r="AD35" s="7"/>
       <c r="AE35" s="7"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>210</v>
       </c>
@@ -4030,7 +4033,7 @@
       <c r="AD36" s="7"/>
       <c r="AE36" s="7"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>211</v>
       </c>
@@ -4082,7 +4085,7 @@
       <c r="AD37" s="7"/>
       <c r="AE37" s="7"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>212</v>
       </c>
@@ -4134,7 +4137,7 @@
       <c r="AD38" s="7"/>
       <c r="AE38" s="7"/>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>213</v>
       </c>
@@ -4186,7 +4189,7 @@
       <c r="AD39" s="7"/>
       <c r="AE39" s="7"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>214</v>
       </c>
@@ -4238,7 +4241,7 @@
       <c r="AD40" s="7"/>
       <c r="AE40" s="7"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>215</v>
       </c>
@@ -4290,7 +4293,7 @@
       <c r="AD41" s="7"/>
       <c r="AE41" s="7"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>216</v>
       </c>
@@ -4342,7 +4345,7 @@
       <c r="AD42" s="7"/>
       <c r="AE42" s="7"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>217</v>
       </c>
@@ -4394,7 +4397,7 @@
       <c r="AD43" s="7"/>
       <c r="AE43" s="7"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>218</v>
       </c>
@@ -4446,7 +4449,7 @@
       <c r="AD44" s="7"/>
       <c r="AE44" s="7"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>219</v>
       </c>
@@ -4498,7 +4501,7 @@
       <c r="AD45" s="7"/>
       <c r="AE45" s="7"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>220</v>
       </c>
@@ -4550,7 +4553,7 @@
       <c r="AD46" s="7"/>
       <c r="AE46" s="7"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>221</v>
       </c>
@@ -4602,7 +4605,7 @@
       <c r="AD47" s="7"/>
       <c r="AE47" s="7"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>222</v>
       </c>
@@ -4654,7 +4657,7 @@
       <c r="AD48" s="7"/>
       <c r="AE48" s="7"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>223</v>
       </c>
@@ -4706,7 +4709,7 @@
       <c r="AD49" s="7"/>
       <c r="AE49" s="7"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>224</v>
       </c>
@@ -4758,7 +4761,7 @@
       <c r="AD50" s="7"/>
       <c r="AE50" s="7"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>225</v>
       </c>
@@ -4810,7 +4813,7 @@
       <c r="AD51" s="7"/>
       <c r="AE51" s="7"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>226</v>
       </c>
@@ -4862,7 +4865,7 @@
       <c r="AD52" s="7"/>
       <c r="AE52" s="7"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>227</v>
       </c>
@@ -4914,7 +4917,7 @@
       <c r="AD53" s="7"/>
       <c r="AE53" s="7"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>228</v>
       </c>
@@ -4950,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>229</v>
       </c>
@@ -4986,7 +4989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>230</v>
       </c>
@@ -5022,7 +5025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>231</v>
       </c>
@@ -5058,7 +5061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>232</v>
       </c>
@@ -5094,7 +5097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>233</v>
       </c>
@@ -5130,7 +5133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>234</v>
       </c>
@@ -5166,7 +5169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>235</v>
       </c>
@@ -5202,7 +5205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>236</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>237</v>
       </c>
@@ -5274,7 +5277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>238</v>
       </c>
@@ -5310,7 +5313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>239</v>
       </c>
@@ -5346,7 +5349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>240</v>
       </c>
@@ -5382,7 +5385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>241</v>
       </c>
@@ -5418,7 +5421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>242</v>
       </c>
@@ -5454,7 +5457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>243</v>
       </c>
@@ -5490,7 +5493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>244</v>
       </c>
@@ -5526,7 +5529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>245</v>
       </c>
@@ -5562,7 +5565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>246</v>
       </c>
@@ -5598,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>247</v>
       </c>
@@ -5634,7 +5637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>248</v>
       </c>
@@ -5670,7 +5673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>249</v>
       </c>
@@ -5706,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>250</v>
       </c>
@@ -5742,7 +5745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>251</v>
       </c>
@@ -5778,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>252</v>
       </c>
@@ -5814,7 +5817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>253</v>
       </c>
@@ -5850,7 +5853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>254</v>
       </c>
@@ -5886,7 +5889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>255</v>
       </c>
@@ -5922,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>256</v>
       </c>
@@ -5958,7 +5961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>257</v>
       </c>
@@ -5994,7 +5997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>258</v>
       </c>
@@ -6030,7 +6033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>259</v>
       </c>
@@ -6066,7 +6069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>260</v>
       </c>
@@ -6102,7 +6105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>261</v>
       </c>
@@ -6138,7 +6141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>262</v>
       </c>
@@ -6174,7 +6177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>263</v>
       </c>
@@ -6227,13 +6230,13 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -6243,7 +6246,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="10">
         <v>1</v>
@@ -6265,7 +6268,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -6294,7 +6297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -6321,7 +6324,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -6333,7 +6336,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6360,7 +6363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -6387,7 +6390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -6414,7 +6417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>12</v>
       </c>
@@ -6441,7 +6444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
@@ -6468,7 +6471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>16</v>
       </c>
@@ -6495,7 +6498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>17</v>
       </c>
@@ -6522,7 +6525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>18</v>
       </c>
@@ -6549,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
@@ -6576,7 +6579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -6603,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>21</v>
       </c>
@@ -6630,7 +6633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>22</v>
       </c>
@@ -6657,7 +6660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>23</v>
       </c>
@@ -6684,7 +6687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>24</v>
       </c>
@@ -6711,7 +6714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>25</v>
       </c>
@@ -6738,7 +6741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>26</v>
       </c>
@@ -6765,7 +6768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>27</v>
       </c>
@@ -6792,7 +6795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>28</v>
       </c>
@@ -6819,7 +6822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>29</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>30</v>
       </c>
@@ -6873,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>31</v>
       </c>
@@ -6900,7 +6903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>32</v>
       </c>
@@ -6927,7 +6930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>33</v>
       </c>
@@ -6954,7 +6957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>34</v>
       </c>
@@ -6981,7 +6984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>35</v>
       </c>
@@ -7008,7 +7011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>36</v>
       </c>
@@ -7035,7 +7038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>37</v>
       </c>
@@ -7062,7 +7065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>38</v>
       </c>
@@ -7089,7 +7092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>39</v>
       </c>
@@ -7116,7 +7119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>40</v>
       </c>
@@ -7143,7 +7146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>42</v>
       </c>
@@ -7170,7 +7173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>43</v>
       </c>
@@ -7197,7 +7200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>44</v>
       </c>
@@ -7224,7 +7227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>45</v>
       </c>
@@ -7251,7 +7254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>50</v>
       </c>
@@ -7278,7 +7281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>54</v>
       </c>
@@ -7305,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>55</v>
       </c>
@@ -7332,7 +7335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>56</v>
       </c>
@@ -7359,7 +7362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>57</v>
       </c>
@@ -7386,7 +7389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>58</v>
       </c>
@@ -7413,7 +7416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>59</v>
       </c>
@@ -7440,7 +7443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60</v>
       </c>
@@ -7467,7 +7470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>61</v>
       </c>
@@ -7494,7 +7497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>62</v>
       </c>
@@ -7521,7 +7524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>63</v>
       </c>
@@ -7548,7 +7551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>64</v>
       </c>
@@ -7575,7 +7578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>65</v>
       </c>
@@ -7602,7 +7605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>66</v>
       </c>
@@ -7629,7 +7632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>67</v>
       </c>
@@ -7656,7 +7659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>68</v>
       </c>
@@ -7683,7 +7686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>70</v>
       </c>
@@ -7710,7 +7713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>71</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>72</v>
       </c>
@@ -7764,7 +7767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>73</v>
       </c>
@@ -7791,7 +7794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>74</v>
       </c>
@@ -7818,7 +7821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>75</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>76</v>
       </c>
@@ -7872,7 +7875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>77</v>
       </c>
@@ -7899,7 +7902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>78</v>
       </c>
@@ -7926,7 +7929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>79</v>
       </c>
@@ -7953,7 +7956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>88</v>
       </c>
@@ -7980,7 +7983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>93</v>
       </c>
@@ -8007,7 +8010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>94</v>
       </c>
@@ -8034,7 +8037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>95</v>
       </c>
@@ -8061,7 +8064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>96</v>
       </c>
@@ -8088,7 +8091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>97</v>
       </c>
@@ -8115,7 +8118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>98</v>
       </c>
@@ -8142,7 +8145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>99</v>
       </c>
@@ -8169,7 +8172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>100</v>
       </c>
@@ -8196,7 +8199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>101</v>
       </c>
@@ -8223,7 +8226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>102</v>
       </c>
@@ -8250,7 +8253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>103</v>
       </c>
@@ -8277,7 +8280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>105</v>
       </c>
@@ -8304,7 +8307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>106</v>
       </c>
@@ -8331,7 +8334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>107</v>
       </c>
@@ -8358,7 +8361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>108</v>
       </c>
@@ -8385,7 +8388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>109</v>
       </c>
@@ -8412,7 +8415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>110</v>
       </c>
@@ -8439,7 +8442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>111</v>
       </c>
@@ -8466,7 +8469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>112</v>
       </c>
@@ -8493,7 +8496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>113</v>
       </c>
@@ -8520,7 +8523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>114</v>
       </c>
@@ -8547,7 +8550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>115</v>
       </c>
@@ -8574,7 +8577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>116</v>
       </c>
@@ -8601,7 +8604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>117</v>
       </c>
@@ -8628,7 +8631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>118</v>
       </c>
@@ -8655,7 +8658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>119</v>
       </c>
@@ -8682,7 +8685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>120</v>
       </c>
@@ -8709,7 +8712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>122</v>
       </c>
@@ -8736,7 +8739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>123</v>
       </c>
@@ -8763,7 +8766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>124</v>
       </c>
@@ -8790,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>125</v>
       </c>
@@ -8817,7 +8820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>126</v>
       </c>
@@ -8844,7 +8847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>127</v>
       </c>
@@ -8871,7 +8874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>128</v>
       </c>
@@ -8898,7 +8901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>130</v>
       </c>
@@ -8925,7 +8928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>131</v>
       </c>
@@ -8952,7 +8955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>132</v>
       </c>
@@ -8979,7 +8982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>133</v>
       </c>
@@ -9006,7 +9009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>134</v>
       </c>
@@ -9033,7 +9036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>135</v>
       </c>
@@ -9060,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>136</v>
       </c>
@@ -9087,7 +9090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>137</v>
       </c>
@@ -9114,7 +9117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>138</v>
       </c>
@@ -9141,7 +9144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>139</v>
       </c>
@@ -9168,7 +9171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>140</v>
       </c>
@@ -9195,7 +9198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>141</v>
       </c>
@@ -9222,7 +9225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>142</v>
       </c>
@@ -9249,7 +9252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>143</v>
       </c>
@@ -9276,7 +9279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>144</v>
       </c>
@@ -9303,7 +9306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>355</v>
       </c>
@@ -9330,7 +9333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>356</v>
       </c>
@@ -9357,7 +9360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>357</v>
       </c>
@@ -9384,7 +9387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>358</v>
       </c>
@@ -9411,7 +9414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>359</v>
       </c>
@@ -9438,7 +9441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>362</v>
       </c>
@@ -9465,7 +9468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>366</v>
       </c>

</xml_diff>